<commit_message>
personalization also ith input field
</commit_message>
<xml_diff>
--- a/SheetsClient/ToDo.xlsx
+++ b/SheetsClient/ToDo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Adjust slider that does not reposition if, after slideing, the weight of the item is unchanged</t>
   </si>
@@ -114,21 +114,12 @@
     <t>Unsubscribe change events on Destroy</t>
   </si>
   <si>
-    <t>Close</t>
-  </si>
-  <si>
     <t>When no search selection criteria is selected retrieve all sheets from Factory and not like now where no sheets are shown</t>
   </si>
   <si>
-    <t>Add a service on the server to be call when an error on the client is cought</t>
-  </si>
-  <si>
     <t>ask if session is a good thing</t>
   </si>
   <si>
-    <t>how to forse reload of a page via router link</t>
-  </si>
-  <si>
     <t>how to format a monetary amount input</t>
   </si>
   <si>
@@ -136,6 +127,15 @@
   </si>
   <si>
     <t>Which component html5 as free text for comment on personalization of sheets</t>
+  </si>
+  <si>
+    <t>Add a service on the server to call when an error on the client is cought</t>
+  </si>
+  <si>
+    <t>Centralized error management on the client</t>
+  </si>
+  <si>
+    <t>how to force reload of a page via router link</t>
   </si>
 </sst>
 </file>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -635,18 +635,18 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
+      <c r="C15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -686,14 +686,14 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -710,19 +710,30 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>29</v>
       </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
         <v>12</v>
       </c>
     </row>
@@ -760,31 +771,31 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -792,10 +803,10 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>